<commit_message>
parameterization for q ilex
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/src/3D-CMCC_FUNCTIONS.xlsx
+++ b/software/3D-CMCC-Forest-Model/src/3D-CMCC_FUNCTIONS.xlsx
@@ -16,6 +16,163 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Autore</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+parameter
+it is the crown diameter to dbh maximum ratio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+parameter
+it is the crown diameter to dbh minimum ratio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+potential maximum stand  density</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+potential minimum stand  density</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+effective stand density
+in this case I use an average stand density between maximum and minimum to check function</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autore:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I don't know why it exceeds of 628.28973 meters...</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -160,13 +317,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -616,8 +786,8 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100553856"/>
-        <c:axId val="100555392"/>
+        <c:axId val="90915584"/>
+        <c:axId val="90917120"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1019,23 +1189,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100562816"/>
-        <c:axId val="100561280"/>
+        <c:axId val="90924544"/>
+        <c:axId val="90923008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100553856"/>
+        <c:axId val="90915584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100555392"/>
+        <c:crossAx val="90917120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100555392"/>
+        <c:axId val="90917120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,24 +1213,24 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100553856"/>
+        <c:crossAx val="90915584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100561280"/>
+        <c:axId val="90923008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100562816"/>
+        <c:crossAx val="90924544"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100562816"/>
+        <c:axId val="90924544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1238,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="100561280"/>
+        <c:crossAx val="90923008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1080,7 +1250,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2999,11 +3169,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102456320"/>
-        <c:axId val="102458112"/>
+        <c:axId val="93735552"/>
+        <c:axId val="93737344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102456320"/>
+        <c:axId val="93735552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000032E-2"/>
@@ -3012,12 +3182,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102458112"/>
+        <c:crossAx val="93737344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102458112"/>
+        <c:axId val="93737344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,7 +3195,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102456320"/>
+        <c:crossAx val="93735552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0000000000000005E-2"/>
@@ -3038,7 +3208,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4081,23 +4251,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102311808"/>
-        <c:axId val="102313344"/>
+        <c:axId val="94971392"/>
+        <c:axId val="94972928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102311808"/>
+        <c:axId val="94971392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102313344"/>
+        <c:crossAx val="94972928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102313344"/>
+        <c:axId val="94972928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4105,7 +4275,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102311808"/>
+        <c:crossAx val="94971392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4118,7 +4288,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5338,30 +5508,66 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="57245696"/>
-        <c:axId val="106021248"/>
+        <c:axId val="95014912"/>
+        <c:axId val="95016448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57245696"/>
+        <c:axId val="95014912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>dbh (cm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106021248"/>
+        <c:crossAx val="95016448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106021248"/>
+        <c:axId val="95016448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>crown area (m^2)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57245696"/>
+        <c:crossAx val="95014912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5374,7 +5580,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5567,24 +5773,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="100181504"/>
-        <c:axId val="100183040"/>
+        <c:axId val="93291648"/>
+        <c:axId val="93293184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100181504"/>
+        <c:axId val="93291648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100183040"/>
+        <c:crossAx val="93293184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100183040"/>
+        <c:axId val="93293184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5592,7 +5798,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100181504"/>
+        <c:crossAx val="93291648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5604,7 +5810,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5978,23 +6184,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101859328"/>
-        <c:axId val="101860864"/>
+        <c:axId val="93310336"/>
+        <c:axId val="90977408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101859328"/>
+        <c:axId val="93310336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101860864"/>
+        <c:crossAx val="90977408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101860864"/>
+        <c:axId val="90977408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6002,7 +6208,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101859328"/>
+        <c:crossAx val="93310336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6014,7 +6220,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6124,23 +6330,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101889536"/>
-        <c:axId val="101891072"/>
+        <c:axId val="91010176"/>
+        <c:axId val="91011712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101889536"/>
+        <c:axId val="91010176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101891072"/>
+        <c:crossAx val="91011712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101891072"/>
+        <c:axId val="91011712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6148,7 +6354,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101889536"/>
+        <c:crossAx val="91010176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6160,7 +6366,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6327,22 +6533,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102075392"/>
-        <c:axId val="102081280"/>
+        <c:axId val="93551232"/>
+        <c:axId val="93553024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102075392"/>
+        <c:axId val="93551232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102081280"/>
+        <c:crossAx val="93553024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102081280"/>
+        <c:axId val="93553024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6350,7 +6556,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102075392"/>
+        <c:crossAx val="93551232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6362,7 +6568,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6529,22 +6735,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102093184"/>
-        <c:axId val="102094720"/>
+        <c:axId val="93577216"/>
+        <c:axId val="93578752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102093184"/>
+        <c:axId val="93577216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102094720"/>
+        <c:crossAx val="93578752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102094720"/>
+        <c:axId val="93578752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6552,7 +6758,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102093184"/>
+        <c:crossAx val="93577216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6564,7 +6770,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6882,22 +7088,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102251136"/>
-        <c:axId val="102261120"/>
+        <c:axId val="93604096"/>
+        <c:axId val="93605888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102251136"/>
+        <c:axId val="93604096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102261120"/>
+        <c:crossAx val="93605888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102261120"/>
+        <c:axId val="93605888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6905,7 +7111,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102251136"/>
+        <c:crossAx val="93604096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6917,7 +7123,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7600,23 +7806,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="102285696"/>
-        <c:axId val="102287232"/>
+        <c:axId val="93638656"/>
+        <c:axId val="93640192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102285696"/>
+        <c:axId val="93638656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102287232"/>
+        <c:crossAx val="93640192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102287232"/>
+        <c:axId val="93640192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7624,7 +7830,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102285696"/>
+        <c:crossAx val="93638656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7636,7 +7842,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7829,24 +8035,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="102192256"/>
-        <c:axId val="102193792"/>
+        <c:axId val="93664000"/>
+        <c:axId val="93665536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102192256"/>
+        <c:axId val="93664000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102193792"/>
+        <c:crossAx val="93665536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102193792"/>
+        <c:axId val="93665536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7854,7 +8060,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102192256"/>
+        <c:crossAx val="93664000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7866,7 +8072,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -17491,7 +17697,7 @@
   <dimension ref="A1:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20859,5 +21065,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some new calibration for fagus
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/src/3D-CMCC_FUNCTIONS.xlsx
+++ b/software/3D-CMCC-Forest-Model/src/3D-CMCC_FUNCTIONS.xlsx
@@ -143,7 +143,7 @@
           </rPr>
           <t xml:space="preserve">
 effective stand density
-in this case I use an average stand density between maximum and minimum to check function</t>
+in this case I use a RANDOM stand density between maximum and minimum to check function</t>
         </r>
       </text>
     </comment>
@@ -310,7 +310,7 @@
     <t>CROWN AREA</t>
   </si>
   <si>
-    <t>AVERAGE DENSITY</t>
+    <t>RANDOM DENSITY</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90915584"/>
-        <c:axId val="90917120"/>
+        <c:axId val="295799808"/>
+        <c:axId val="295817984"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1189,23 +1189,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90924544"/>
-        <c:axId val="90923008"/>
+        <c:axId val="295825408"/>
+        <c:axId val="295819520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90915584"/>
+        <c:axId val="295799808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90917120"/>
+        <c:crossAx val="295817984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90917120"/>
+        <c:axId val="295817984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,24 +1213,24 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90915584"/>
+        <c:crossAx val="295799808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90923008"/>
+        <c:axId val="295819520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="r"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90924544"/>
+        <c:crossAx val="295825408"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90924544"/>
+        <c:axId val="295825408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,7 +1238,7 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="90923008"/>
+        <c:crossAx val="295819520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1250,7 +1250,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3169,11 +3169,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93735552"/>
-        <c:axId val="93737344"/>
+        <c:axId val="297383040"/>
+        <c:axId val="297384576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93735552"/>
+        <c:axId val="297383040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6.0000000000000032E-2"/>
@@ -3182,12 +3182,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93737344"/>
+        <c:crossAx val="297384576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93737344"/>
+        <c:axId val="297384576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3195,7 +3195,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93735552"/>
+        <c:crossAx val="297383040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0000000000000005E-2"/>
@@ -3208,7 +3208,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4251,23 +4251,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="94971392"/>
-        <c:axId val="94972928"/>
+        <c:axId val="297582592"/>
+        <c:axId val="297584128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94971392"/>
+        <c:axId val="297582592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94972928"/>
+        <c:crossAx val="297584128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94972928"/>
+        <c:axId val="297584128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4275,7 +4275,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94971392"/>
+        <c:crossAx val="297582592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4288,7 +4288,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4318,7 +4318,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -4521,184 +4523,184 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>3.4618499999999996E-2</c:v>
+                  <c:v>3.0834203822136325E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13847399999999999</c:v>
+                  <c:v>0.17351763718985783</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31156650000000002</c:v>
+                  <c:v>0.27209479110361567</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55389599999999994</c:v>
+                  <c:v>0.51354605194362735</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86546250000000002</c:v>
+                  <c:v>0.7414231936772947</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2462660000000001</c:v>
+                  <c:v>1.1168163786435776</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6963064999999999</c:v>
+                  <c:v>1.5741465720334704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2155839999999998</c:v>
+                  <c:v>2.7986826982737436</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8040984999999998</c:v>
+                  <c:v>2.9410645016645027</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4618500000000001</c:v>
+                  <c:v>4.011506277500251</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.1888385000000001</c:v>
+                  <c:v>4.3680846780776879</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.9850640000000004</c:v>
+                  <c:v>5.4512519131254074</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.8505265</c:v>
+                  <c:v>4.872052058785421</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.7852259999999998</c:v>
+                  <c:v>7.359980063811749</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.7891624999999998</c:v>
+                  <c:v>8.295139170641507</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.8623359999999991</c:v>
+                  <c:v>10.420428874353902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.0047465</c:v>
+                  <c:v>11.35771253676794</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.216393999999999</c:v>
+                  <c:v>11.162918695936337</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12.497278499999998</c:v>
+                  <c:v>10.32809445674568</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.8474</c:v>
+                  <c:v>17.826894439571408</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15.2667585</c:v>
+                  <c:v>17.018844939334951</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16.755354000000001</c:v>
+                  <c:v>21.56877307874003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18.3131865</c:v>
+                  <c:v>14.291427821034301</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>19.940256000000002</c:v>
+                  <c:v>15.086695570728462</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>21.6365625</c:v>
+                  <c:v>25.197866051523647</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.402106</c:v>
+                  <c:v>21.004034571903674</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25.236886500000001</c:v>
+                  <c:v>25.062372298509196</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>27.140903999999999</c:v>
+                  <c:v>23.561319196002323</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29.114158499999998</c:v>
+                  <c:v>34.118460967938617</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>31.156649999999999</c:v>
+                  <c:v>27.726649163323305</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>33.268378499999997</c:v>
+                  <c:v>33.959570787930588</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>35.449343999999996</c:v>
+                  <c:v>30.879444870024404</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>37.699546499999997</c:v>
+                  <c:v>48.926189307396236</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>40.018985999999998</c:v>
+                  <c:v>29.923786209388084</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42.407662499999994</c:v>
+                  <c:v>38.138998479709805</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>44.865575999999997</c:v>
+                  <c:v>39.961831818887092</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>47.392726499999995</c:v>
+                  <c:v>36.323486505430722</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>49.989113999999994</c:v>
+                  <c:v>51.832064094216932</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>52.654738500000001</c:v>
+                  <c:v>59.760076782294256</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>55.389600000000002</c:v>
+                  <c:v>48.513411425126961</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>58.193698499999996</c:v>
+                  <c:v>44.948690056827985</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>61.067034</c:v>
+                  <c:v>55.829320701385811</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>64.009606500000004</c:v>
+                  <c:v>82.506717231599666</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>67.021416000000002</c:v>
+                  <c:v>69.01135185990934</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>70.102462499999987</c:v>
+                  <c:v>63.927476332692407</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>73.252746000000002</c:v>
+                  <c:v>88.439228807082486</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>76.472266499999989</c:v>
+                  <c:v>85.708907425941348</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>79.761024000000006</c:v>
+                  <c:v>81.142250827377296</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>83.119018499999996</c:v>
+                  <c:v>93.977726763414566</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>86.546250000000001</c:v>
+                  <c:v>107.69635396955633</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>90.042718499999992</c:v>
+                  <c:v>70.9662660207198</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>93.608423999999999</c:v>
+                  <c:v>120.10912026432382</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>97.243366499999993</c:v>
+                  <c:v>81.834177685327191</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>100.947546</c:v>
+                  <c:v>88.891099525243717</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>104.72096249999998</c:v>
+                  <c:v>78.67043622823752</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>108.563616</c:v>
+                  <c:v>102.86843648220105</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>112.47550649999998</c:v>
+                  <c:v>87.871549433902047</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>116.45663399999999</c:v>
+                  <c:v>135.76997696192004</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>120.50699849999998</c:v>
+                  <c:v>148.75738035684466</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>124.6266</c:v>
+                  <c:v>132.62606554212701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5508,11 +5510,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95014912"/>
-        <c:axId val="95016448"/>
+        <c:axId val="297634048"/>
+        <c:axId val="297640320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95014912"/>
+        <c:axId val="297634048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5537,12 +5539,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95016448"/>
+        <c:crossAx val="297640320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95016448"/>
+        <c:axId val="297640320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5567,7 +5569,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95014912"/>
+        <c:crossAx val="297634048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5580,7 +5582,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5773,24 +5775,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93291648"/>
-        <c:axId val="93293184"/>
+        <c:axId val="296209792"/>
+        <c:axId val="296215680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93291648"/>
+        <c:axId val="296209792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93293184"/>
+        <c:crossAx val="296215680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93293184"/>
+        <c:axId val="296215680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5798,7 +5800,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93291648"/>
+        <c:crossAx val="296209792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5810,7 +5812,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6184,23 +6186,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93310336"/>
-        <c:axId val="90977408"/>
+        <c:axId val="296867328"/>
+        <c:axId val="296868864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93310336"/>
+        <c:axId val="296867328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90977408"/>
+        <c:crossAx val="296868864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90977408"/>
+        <c:axId val="296868864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6208,7 +6210,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93310336"/>
+        <c:crossAx val="296867328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6220,7 +6222,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6330,23 +6332,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91010176"/>
-        <c:axId val="91011712"/>
+        <c:axId val="296893440"/>
+        <c:axId val="296899328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91010176"/>
+        <c:axId val="296893440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91011712"/>
+        <c:crossAx val="296899328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91011712"/>
+        <c:axId val="296899328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6354,7 +6356,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91010176"/>
+        <c:crossAx val="296893440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6366,7 +6368,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6533,22 +6535,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93551232"/>
-        <c:axId val="93553024"/>
+        <c:axId val="296944384"/>
+        <c:axId val="296945920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93551232"/>
+        <c:axId val="296944384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93553024"/>
+        <c:crossAx val="296945920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93553024"/>
+        <c:axId val="296945920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6556,7 +6558,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93551232"/>
+        <c:crossAx val="296944384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6568,7 +6570,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6735,22 +6737,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93577216"/>
-        <c:axId val="93578752"/>
+        <c:axId val="296970112"/>
+        <c:axId val="296971648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93577216"/>
+        <c:axId val="296970112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93578752"/>
+        <c:crossAx val="296971648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93578752"/>
+        <c:axId val="296971648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6758,7 +6760,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93577216"/>
+        <c:crossAx val="296970112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6770,7 +6772,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7088,22 +7090,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93604096"/>
-        <c:axId val="93605888"/>
+        <c:axId val="297190144"/>
+        <c:axId val="297191680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93604096"/>
+        <c:axId val="297190144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93605888"/>
+        <c:crossAx val="297191680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93605888"/>
+        <c:axId val="297191680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7111,7 +7113,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93604096"/>
+        <c:crossAx val="297190144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7123,7 +7125,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7806,23 +7808,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93638656"/>
-        <c:axId val="93640192"/>
+        <c:axId val="297208064"/>
+        <c:axId val="297238528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93638656"/>
+        <c:axId val="297208064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93640192"/>
+        <c:crossAx val="297238528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93640192"/>
+        <c:axId val="297238528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7830,7 +7832,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93638656"/>
+        <c:crossAx val="297208064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7842,7 +7844,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8035,24 +8037,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="93664000"/>
-        <c:axId val="93665536"/>
+        <c:axId val="297253888"/>
+        <c:axId val="297280256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93664000"/>
+        <c:axId val="297253888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93665536"/>
+        <c:crossAx val="297280256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93665536"/>
+        <c:axId val="297280256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8060,7 +8062,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93664000"/>
+        <c:crossAx val="297253888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8072,7 +8074,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -17696,8 +17698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17797,24 +17799,24 @@
         <v>221048.5320432139</v>
       </c>
       <c r="J2" s="2">
-        <f>P2</f>
-        <v>307011.85006001929</v>
+        <f ca="1">P2</f>
+        <v>340853</v>
       </c>
       <c r="K2" s="2">
-        <f>((C2-B2)/(H2-I2))*(J2-I2)+B2</f>
-        <v>0.21</v>
+        <f ca="1">((C2-B2)/(H2-I2))*(J2-I2)+B2</f>
+        <v>0.19818991028241897</v>
       </c>
       <c r="L2" s="2">
-        <f>((((K2*A2)/2)^2)*3.14)</f>
-        <v>3.4618499999999996E-2</v>
+        <f ca="1">((((K2*A2)/2)^2)*3.14)</f>
+        <v>3.0834203822136325E-2</v>
       </c>
       <c r="M2" s="2">
-        <f>L2*J2</f>
-        <v>10628.289731302777</v>
+        <f ca="1">L2*J2</f>
+        <v>10509.930875386633</v>
       </c>
       <c r="P2" s="2">
-        <f>AVERAGE(H2:I2)</f>
-        <v>307011.85006001929</v>
+        <f ca="1">RANDBETWEEN(I2,H2)</f>
+        <v>340853</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -17852,24 +17854,24 @@
         <v>55262.133010803474</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J61" si="6">P3</f>
-        <v>76752.962515004823</v>
+        <f t="shared" ref="J3:J61" ca="1" si="6">P3</f>
+        <v>58790</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" ref="K3:K61" si="7">((C3-B3)/(H3-I3))*(J3-I3)+B3</f>
-        <v>0.21</v>
+        <f t="shared" ref="K3:K61" ca="1" si="7">((C3-B3)/(H3-I3))*(J3-I3)+B3</f>
+        <v>0.23507529434100227</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L61" si="8">((((K3*A3)/2)^2)*3.14)</f>
-        <v>0.13847399999999999</v>
+        <f t="shared" ref="L3:L61" ca="1" si="8">((((K3*A3)/2)^2)*3.14)</f>
+        <v>0.17351763718985783</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ref="M3:M61" si="9">L3*J3</f>
-        <v>10628.289731302777</v>
+        <f t="shared" ref="M3:M61" ca="1" si="9">L3*J3</f>
+        <v>10201.101890391741</v>
       </c>
       <c r="P3" s="2">
-        <f t="shared" ref="P3:P61" si="10">AVERAGE(H3:I3)</f>
-        <v>76752.962515004823</v>
+        <f t="shared" ref="P3:P61" ca="1" si="10">RANDBETWEEN(I3,H3)</f>
+        <v>58790</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -17907,24 +17909,24 @@
         <v>24560.948004801547</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="6"/>
-        <v>34112.427784446591</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>38491</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19624745385039344</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="8"/>
-        <v>0.31156650000000002</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.27209479110361567</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10473.200604369271</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" si="10"/>
-        <v>34112.427784446591</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>38491</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -17962,24 +17964,24 @@
         <v>13815.533252700869</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="6"/>
-        <v>19188.240628751206</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>20584</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.2022063908925846</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="8"/>
-        <v>0.55389599999999994</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.51354605194362735</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10570.831933207624</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" si="10"/>
-        <v>19188.240628751206</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>20584</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -18017,24 +18019,24 @@
         <v>8841.9412817285574</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="6"/>
-        <v>12280.474002400775</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>14072</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19436955984020135</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="8"/>
-        <v>0.86546250000000002</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.7414231936772947</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10433.307181426891</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" si="10"/>
-        <v>12280.474002400775</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>14072</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -18072,24 +18074,24 @@
         <v>6140.2370012003867</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="6"/>
-        <v>8528.1069461116476</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>9420</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19879470313126918</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="8"/>
-        <v>1.2462660000000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.1168163786435776</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10520.410286822502</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" si="10"/>
-        <v>8528.1069461116476</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>9420</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -18127,24 +18129,24 @@
         <v>4511.1945314941622</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="6"/>
-        <v>6265.5479604085576</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6716</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.20229712726921534</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="8"/>
-        <v>1.6963064999999999</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.5741465720334704</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10571.968377776788</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" si="10"/>
-        <v>6265.5479604085576</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>6716</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -18182,24 +18184,24 @@
         <v>3453.8833131752172</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="6"/>
-        <v>4797.0601571878015</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>3632</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23602174454647357</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="8"/>
-        <v>2.2155839999999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.7986826982737436</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10164.815560130237</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" si="10"/>
-        <v>4797.0601571878015</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>3632</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -18237,24 +18239,24 @@
         <v>2728.9942227557272</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="6"/>
-        <v>3790.2697538273997</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>3611</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21506757430786252</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="8"/>
-        <v>2.8040984999999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.9410645016645027</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10620.183915510519</v>
       </c>
       <c r="P10" s="2">
-        <f t="shared" si="10"/>
-        <v>3790.2697538273997</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>3611</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -18292,24 +18294,24 @@
         <v>2210.4853204321394</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="6"/>
-        <v>3070.1185006001938</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2610</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22605749444816367</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="8"/>
-        <v>3.4618500000000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>4.011506277500251</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10470.031384275655</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" si="10"/>
-        <v>3070.1185006001938</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>2610</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -18347,24 +18349,24 @@
         <v>1826.8473722579668</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="6"/>
-        <v>2537.2880170249532</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2432</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21444603012794206</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="8"/>
-        <v>4.1888385000000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>4.3680846780776879</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10623.181937084937</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" si="10"/>
-        <v>2537.2880170249532</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>2432</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -18402,24 +18404,24 @@
         <v>1535.0592503000967</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="6"/>
-        <v>2132.0267365279119</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1941</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21959985632056744</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="8"/>
-        <v>4.9850640000000004</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>5.4512519131254074</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10580.879963376416</v>
       </c>
       <c r="P13" s="2">
-        <f t="shared" si="10"/>
-        <v>2132.0267365279119</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>1941</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -18457,24 +18459,24 @@
         <v>1307.9794795456442</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="6"/>
-        <v>1816.6381660356174</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2128</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19163630098723261</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="8"/>
-        <v>5.8505265</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>4.872052058785421</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10367.726781095376</v>
       </c>
       <c r="P14" s="2">
-        <f t="shared" si="10"/>
-        <v>1816.6381660356174</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>2128</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -18512,24 +18514,24 @@
         <v>1127.7986328735406</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="6"/>
-        <v>1566.3869901021394</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1439</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21871343171809801</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="8"/>
-        <v>6.7852259999999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>7.359980063811749</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10591.011311825107</v>
       </c>
       <c r="P15" s="2">
-        <f t="shared" si="10"/>
-        <v>1566.3869901021394</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>1439</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -18567,24 +18569,24 @@
         <v>982.43792019206205</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="6"/>
-        <v>1364.4971113778638</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1279</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21671339258551839</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="8"/>
-        <v>7.7891624999999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8.295139170641507</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10609.482999250487</v>
       </c>
       <c r="P16" s="2">
-        <f t="shared" si="10"/>
-        <v>1364.4971113778638</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>1279</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -18622,24 +18624,24 @@
         <v>863.47082829380429</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="6"/>
-        <v>1199.2650392969504</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1001</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22771308433561049</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="8"/>
-        <v>8.8623359999999991</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>10.420428874353902</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10430.849303228257</v>
       </c>
       <c r="P17" s="2">
-        <f t="shared" si="10"/>
-        <v>1199.2650392969504</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>1001</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -18677,24 +18679,24 @@
         <v>764.87381329831794</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="6"/>
-        <v>1062.3247406921082</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>926</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22374930062110349</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="8"/>
-        <v>10.0047465</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>11.35771253676794</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10517.241809047113</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" si="10"/>
-        <v>1062.3247406921082</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>926</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -18732,24 +18734,24 @@
         <v>682.24855568893179</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="6"/>
-        <v>947.56743845684991</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>952</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.20949880368518353</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="8"/>
-        <v>11.216393999999999</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>11.162918695936337</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10627.098598531393</v>
       </c>
       <c r="P19" s="2">
-        <f t="shared" si="10"/>
-        <v>947.56743845684991</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>952</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -18787,24 +18789,24 @@
         <v>612.32280344380581</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="6"/>
-        <v>850.44833811639705</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1002</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.1909069201135471</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="8"/>
-        <v>12.497278499999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>10.32809445674568</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10348.750645659171</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" si="10"/>
-        <v>850.44833811639705</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>1002</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -18842,24 +18844,24 @@
         <v>552.62133010803484</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="6"/>
-        <v>767.52962515004845</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>565</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23827200668691564</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="8"/>
-        <v>13.8474</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>17.826894439571408</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10072.195358357845</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="10"/>
-        <v>767.52962515004845</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>565</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -18897,24 +18899,24 @@
         <v>501.24383683268456</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="6"/>
-        <v>696.17199560095082</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>620</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22172308753372649</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="8"/>
-        <v>15.2667585</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>17.018844939334951</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10551.68386238767</v>
       </c>
       <c r="P22" s="2">
-        <f t="shared" si="10"/>
-        <v>696.17199560095082</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>620</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -18952,24 +18954,24 @@
         <v>456.71184306449169</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="6"/>
-        <v>634.3220042562383</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>467</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23826223507712466</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="8"/>
-        <v>16.755354000000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>21.56877307874003</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10072.617027771594</v>
       </c>
       <c r="P23" s="2">
-        <f t="shared" si="10"/>
-        <v>634.3220042562383</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>467</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -19007,24 +19009,24 @@
         <v>417.86111917431748</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="6"/>
-        <v>580.36266551988535</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>713</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.1855133404949782</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="8"/>
-        <v>18.3131865</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>14.291427821034301</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10189.788036397456</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="10"/>
-        <v>580.36266551988535</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>713</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -19062,24 +19064,24 @@
         <v>383.76481257502417</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="6"/>
-        <v>533.00668413197798</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>669</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.18266317131058141</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="8"/>
-        <v>19.940256000000002</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>15.086695570728462</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10092.999336817342</v>
       </c>
       <c r="P25" s="2">
-        <f t="shared" si="10"/>
-        <v>533.00668413197798</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>669</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -19117,24 +19119,24 @@
         <v>353.67765126914225</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="6"/>
-        <v>491.21896009603086</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>415</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.2266245968021057</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="8"/>
-        <v>21.6365625</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>25.197866051523647</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10457.114411382314</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="10"/>
-        <v>491.21896009603086</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>415</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -19172,24 +19174,24 @@
         <v>326.99486988641104</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="6"/>
-        <v>454.15954150890434</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>501</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19894965294366937</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="8"/>
-        <v>23.402106</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>21.004034571903674</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10523.02132052374</v>
       </c>
       <c r="P27" s="2">
-        <f t="shared" si="10"/>
-        <v>454.15954150890434</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>501</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -19227,24 +19229,24 @@
         <v>303.22158030619198</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="6"/>
-        <v>421.14108375859996</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>424</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.20927266071573464</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="8"/>
-        <v>25.236886500000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>25.062372298509196</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10626.445854567899</v>
       </c>
       <c r="P28" s="2">
-        <f t="shared" si="10"/>
-        <v>421.14108375859996</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>424</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -19282,24 +19284,24 @@
         <v>281.94965821838514</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="6"/>
-        <v>391.59674752553485</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>444</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19566220422112524</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="8"/>
-        <v>27.140903999999999</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>23.561319196002323</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10461.225723025031</v>
       </c>
       <c r="P29" s="2">
-        <f t="shared" si="10"/>
-        <v>391.59674752553485</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>444</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -19337,24 +19339,24 @@
         <v>262.84010944496305</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="6"/>
-        <v>365.05570756244867</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>306</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22733268952588936</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="8"/>
-        <v>29.114158499999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>34.118460967938617</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10440.249056189217</v>
       </c>
       <c r="P30" s="2">
-        <f t="shared" si="10"/>
-        <v>365.05570756244867</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>306</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -19392,24 +19394,24 @@
         <v>245.60948004801551</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="6"/>
-        <v>341.12427784446595</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>379</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.1981037107246198</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="8"/>
-        <v>31.156649999999999</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>27.726649163323305</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10508.400032899533</v>
       </c>
       <c r="P31" s="2">
-        <f t="shared" si="10"/>
-        <v>341.12427784446595</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -19447,24 +19449,24 @@
         <v>230.01928412405195</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="6"/>
-        <v>319.47122795007215</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>313</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21217029200483056</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="8"/>
-        <v>33.268378499999997</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>33.959570787930588</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10629.345656622274</v>
       </c>
       <c r="P32" s="2">
-        <f t="shared" si="10"/>
-        <v>319.47122795007215</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -19502,24 +19504,24 @@
         <v>215.86770707345107</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="6"/>
-        <v>299.81625982423759</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>339</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19599723084253101</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="8"/>
-        <v>35.449343999999996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>30.879444870024404</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10468.131810938274</v>
       </c>
       <c r="P33" s="2">
-        <f t="shared" si="10"/>
-        <v>299.81625982423759</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -19557,24 +19559,24 @@
         <v>202.98304136199624</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="6"/>
-        <v>281.92089078055039</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>205</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23923346329313741</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="8"/>
-        <v>37.699546499999997</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>48.926189307396236</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10029.868808016228</v>
       </c>
       <c r="P34" s="2">
-        <f t="shared" si="10"/>
-        <v>281.92089078055039</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -19612,24 +19614,24 @@
         <v>191.21845332457949</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="6"/>
-        <v>265.58118517302705</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>336</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.18159108612208291</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="8"/>
-        <v>40.018985999999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>29.923786209388084</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10054.392166354395</v>
       </c>
       <c r="P35" s="2">
-        <f t="shared" si="10"/>
-        <v>265.58118517302705</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>336</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -19667,24 +19669,24 @@
         <v>180.44778125976646</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="6"/>
-        <v>250.62191841634228</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>276</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19915066891651281</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="8"/>
-        <v>42.407662499999994</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>38.138998479709805</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10526.363580399906</v>
       </c>
       <c r="P36" s="2">
-        <f t="shared" si="10"/>
-        <v>250.62191841634228</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -19722,24 +19724,24 @@
         <v>170.56213892223295</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="6"/>
-        <v>236.89185961421248</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>263</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19819165521273882</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="8"/>
-        <v>44.865575999999997</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>39.961831818887092</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10509.961768367306</v>
       </c>
       <c r="P37" s="2">
-        <f t="shared" si="10"/>
-        <v>236.89185961421248</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -19777,24 +19779,24 @@
         <v>161.46715269774577</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="6"/>
-        <v>224.25993430242465</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>279</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.1838472810256124</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" si="8"/>
-        <v>47.392726499999995</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>36.323486505430722</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10134.252735015172</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" si="10"/>
-        <v>224.25993430242465</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -19832,24 +19834,24 @@
         <v>153.08070086095145</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="6"/>
-        <v>212.61208452909926</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>205</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21383600248813237</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="8"/>
-        <v>49.989113999999994</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>51.832064094216932</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10625.573139314471</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="10"/>
-        <v>212.61208452909926</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -19887,24 +19889,24 @@
         <v>145.33105328284941</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="6"/>
-        <v>201.84868511506863</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>176</v>
       </c>
       <c r="K40" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22372068376385842</v>
       </c>
       <c r="L40" s="2">
-        <f t="shared" si="8"/>
-        <v>52.654738500000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>59.760076782294256</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10517.773513683789</v>
       </c>
       <c r="P40" s="2">
-        <f t="shared" si="10"/>
-        <v>201.84868511506863</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -19942,24 +19944,24 @@
         <v>138.15533252700871</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="6"/>
-        <v>191.88240628751211</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>216</v>
       </c>
       <c r="K41" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19653327343678026</v>
       </c>
       <c r="L41" s="2">
-        <f t="shared" si="8"/>
-        <v>55.389600000000002</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>48.513411425126961</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10478.896867827423</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" si="10"/>
-        <v>191.88240628751211</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -19997,24 +19999,24 @@
         <v>131.49823441000234</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" si="6"/>
-        <v>182.6364366805588</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>226</v>
       </c>
       <c r="K42" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.18456095752641952</v>
       </c>
       <c r="L42" s="2">
-        <f t="shared" si="8"/>
-        <v>58.193698499999996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>44.948690056827985</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10158.403952843124</v>
       </c>
       <c r="P42" s="2">
-        <f t="shared" si="10"/>
-        <v>182.6364366805588</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -20052,24 +20054,24 @@
         <v>125.31095920817114</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="6"/>
-        <v>174.04299890023771</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>189</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.20079229936140108</v>
       </c>
       <c r="L43" s="2">
-        <f t="shared" si="8"/>
-        <v>61.067034</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>55.829320701385811</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10551.741612561918</v>
       </c>
       <c r="P43" s="2">
-        <f t="shared" si="10"/>
-        <v>174.04299890023771</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -20107,24 +20109,24 @@
         <v>119.55031478810919</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="6"/>
-        <v>166.0421038723739</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>122</v>
       </c>
       <c r="K44" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.2384192788059086</v>
       </c>
       <c r="L44" s="2">
-        <f t="shared" si="8"/>
-        <v>64.009606500000004</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>82.506717231599666</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10065.819502255159</v>
       </c>
       <c r="P44" s="2">
-        <f t="shared" si="10"/>
-        <v>166.0421038723739</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -20162,24 +20164,24 @@
         <v>114.17796076612292</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="6"/>
-        <v>158.58050106405958</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>154</v>
       </c>
       <c r="K45" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21309475608827211</v>
       </c>
       <c r="L45" s="2">
-        <f t="shared" si="8"/>
-        <v>67.021416000000002</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>69.01135185990934</v>
       </c>
       <c r="M45" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10627.748186426039</v>
       </c>
       <c r="P45" s="2">
-        <f t="shared" si="10"/>
-        <v>158.58050106405958</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -20217,24 +20219,24 @@
         <v>109.1597689102291</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="6"/>
-        <v>151.61079015309599</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>165</v>
       </c>
       <c r="K46" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.20053788852077109</v>
       </c>
       <c r="L46" s="2">
-        <f t="shared" si="8"/>
-        <v>70.102462499999987</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>63.927476332692407</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10548.033594894247</v>
       </c>
       <c r="P46" s="2">
-        <f t="shared" si="10"/>
-        <v>151.61079015309599</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -20272,24 +20274,24 @@
         <v>104.46527979357937</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="6"/>
-        <v>145.09066637997134</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>117</v>
       </c>
       <c r="K47" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23074367931507686</v>
       </c>
       <c r="L47" s="2">
-        <f t="shared" si="8"/>
-        <v>73.252746000000002</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>88.439228807082486</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10347.38977042865</v>
       </c>
       <c r="P47" s="2">
-        <f t="shared" si="10"/>
-        <v>145.09066637997134</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -20327,24 +20329,24 @@
         <v>100.06723949443817</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="6"/>
-        <v>138.98227707560858</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>123</v>
       </c>
       <c r="K48" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22232090066129745</v>
       </c>
       <c r="L48" s="2">
-        <f t="shared" si="8"/>
-        <v>76.472266499999989</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>85.708907425941348</v>
       </c>
       <c r="M48" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10542.195613390786</v>
       </c>
       <c r="P48" s="2">
-        <f t="shared" si="10"/>
-        <v>138.98227707560858</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -20382,24 +20384,24 @@
         <v>95.941203143756042</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="6"/>
-        <v>133.25167103299449</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>131</v>
       </c>
       <c r="K49" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21181048737288333</v>
       </c>
       <c r="L49" s="2">
-        <f t="shared" si="8"/>
-        <v>79.761024000000006</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>81.142250827377296</v>
       </c>
       <c r="M49" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10629.634858386426</v>
       </c>
       <c r="P49" s="2">
-        <f t="shared" si="10"/>
-        <v>133.25167103299449</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -20437,24 +20439,24 @@
         <v>92.065194520289026</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="6"/>
-        <v>127.86832572262364</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>112</v>
       </c>
       <c r="K50" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22329631671007777</v>
       </c>
       <c r="L50" s="2">
-        <f t="shared" si="8"/>
-        <v>83.119018499999996</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>93.977726763414566</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10525.505397502431</v>
       </c>
       <c r="P50" s="2">
-        <f t="shared" si="10"/>
-        <v>127.86832572262364</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -20492,24 +20494,24 @@
         <v>88.419412817285561</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="6"/>
-        <v>122.80474002400771</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>95</v>
       </c>
       <c r="K51" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23425866695132569</v>
       </c>
       <c r="L51" s="2">
-        <f t="shared" si="8"/>
-        <v>86.546250000000001</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>107.69635396955633</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10231.153627107851</v>
       </c>
       <c r="P51" s="2">
-        <f t="shared" si="10"/>
-        <v>122.80474002400771</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -20547,24 +20549,24 @@
         <v>84.985979255368662</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="6"/>
-        <v>118.03608229912317</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>144</v>
       </c>
       <c r="K52" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.18643222080139632</v>
       </c>
       <c r="L52" s="2">
-        <f t="shared" si="8"/>
-        <v>90.042718499999992</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>70.9662660207198</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10219.142306983651</v>
       </c>
       <c r="P52" s="2">
-        <f t="shared" si="10"/>
-        <v>118.03608229912317</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -20602,24 +20604,24 @@
         <v>81.74871747160276</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" si="6"/>
-        <v>113.53988537722608</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>84</v>
       </c>
       <c r="K53" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23787555851825215</v>
       </c>
       <c r="L53" s="2">
-        <f t="shared" si="8"/>
-        <v>93.608423999999999</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>120.10912026432382</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10089.1661022032</v>
       </c>
       <c r="P53" s="2">
-        <f t="shared" si="10"/>
-        <v>113.53988537722608</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -20657,24 +20659,24 @@
         <v>78.692962635533632</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="6"/>
-        <v>109.29578143824115</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>127</v>
       </c>
       <c r="K54" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19264452172602559</v>
       </c>
       <c r="L54" s="2">
-        <f t="shared" si="8"/>
-        <v>97.243366499999993</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>81.834177685327191</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10392.940566036554</v>
       </c>
       <c r="P54" s="2">
-        <f t="shared" si="10"/>
-        <v>109.29578143824115</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -20712,24 +20714,24 @@
         <v>75.805395076547995</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="6"/>
-        <v>105.28527093964999</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>118</v>
       </c>
       <c r="K55" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.19706094036549435</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" si="8"/>
-        <v>100.947546</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>88.891099525243717</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10489.149743978758</v>
       </c>
       <c r="P55" s="2">
-        <f t="shared" si="10"/>
-        <v>105.28527093964999</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -20767,24 +20769,24 @@
         <v>73.07389489031867</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" si="6"/>
-        <v>101.49152068099812</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>128</v>
       </c>
       <c r="K56" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.18201545317586357</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" si="8"/>
-        <v>104.72096249999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>78.67043622823752</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10069.815837214403</v>
       </c>
       <c r="P56" s="2">
-        <f t="shared" si="10"/>
-        <v>101.49152068099812</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -20822,24 +20824,24 @@
         <v>70.487414554596285</v>
       </c>
       <c r="J57" s="2">
-        <f t="shared" si="6"/>
-        <v>97.899186881383713</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>103</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.20441756659386268</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="8"/>
-        <v>108.563616</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>102.86843648220105</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10595.448957666707</v>
       </c>
       <c r="P57" s="2">
-        <f t="shared" si="10"/>
-        <v>97.899186881383713</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -20877,24 +20879,24 @@
         <v>68.035867049311761</v>
       </c>
       <c r="J58" s="2">
-        <f t="shared" si="6"/>
-        <v>94.494259790710771</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>116</v>
       </c>
       <c r="K58" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.18561559341171974</v>
       </c>
       <c r="L58" s="2">
-        <f t="shared" si="8"/>
-        <v>112.47550649999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>87.871549433902047</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302777</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10193.099734332638</v>
       </c>
       <c r="P58" s="2">
-        <f t="shared" si="10"/>
-        <v>94.494259790710771</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -20932,24 +20934,24 @@
         <v>65.710027361240762</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" si="6"/>
-        <v>91.263926890612169</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>77</v>
       </c>
       <c r="K59" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.22674569496630134</v>
       </c>
       <c r="L59" s="2">
-        <f t="shared" si="8"/>
-        <v>116.45663399999999</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>135.76997696192004</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10454.288226067843</v>
       </c>
       <c r="P59" s="2">
-        <f t="shared" si="10"/>
-        <v>91.263926890612169</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -20987,24 +20989,24 @@
         <v>63.501445574034449</v>
       </c>
       <c r="J60" s="2">
-        <f t="shared" si="6"/>
-        <v>88.196452186158965</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>69</v>
       </c>
       <c r="K60" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.23332024342532559</v>
       </c>
       <c r="L60" s="2">
-        <f t="shared" si="8"/>
-        <v>120.50699849999998</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>148.75738035684466</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302779</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10264.259244622282</v>
       </c>
       <c r="P60" s="2">
-        <f t="shared" si="10"/>
-        <v>88.196452186158965</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -21042,24 +21044,24 @@
         <v>61.402370012003878</v>
       </c>
       <c r="J61" s="2">
-        <f t="shared" si="6"/>
-        <v>85.281069461116488</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>80</v>
       </c>
       <c r="K61" s="2">
-        <f t="shared" si="7"/>
-        <v>0.21</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21663487072112642</v>
       </c>
       <c r="L61" s="2">
-        <f t="shared" si="8"/>
-        <v>124.6266</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>132.62606554212701</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" si="9"/>
-        <v>10628.289731302781</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>10610.08524337016</v>
       </c>
       <c r="P61" s="2">
-        <f t="shared" si="10"/>
-        <v>85.281069461116488</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>